<commit_message>
1. Highlighted portions of the deck to cover in presentation 2. Fixed 26th over winner prediction paramaters in Excel
</commit_message>
<xml_diff>
--- a/IPL_PredictionParameters_AIC.xlsx
+++ b/IPL_PredictionParameters_AIC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\dataScience\springboard\springboardIntro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{270048AA-8215-433C-B412-66CD587A1320}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D04EDA80-E8C6-4663-8A40-8BAB046B56D2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9180" xr2:uid="{EC28E8F2-7017-4161-8F43-E8853987C76B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="45">
   <si>
     <t>Over 0</t>
   </si>
@@ -810,203 +810,203 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1324,165 +1324,160 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EF80A2-B1F7-447D-A99C-78626F568BBD}">
   <dimension ref="A1:AY71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD21" sqref="AD21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AH17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="7.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="5.21875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="5.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" style="1" customWidth="1"/>
+    <col min="9" max="12" width="5.28515625" style="1" customWidth="1"/>
     <col min="13" max="13" width="5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="4.88671875" style="1" customWidth="1"/>
-    <col min="15" max="16" width="5.109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="5.109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="5.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="5.140625" style="1" customWidth="1"/>
     <col min="19" max="19" width="5" style="1" customWidth="1"/>
-    <col min="20" max="20" width="5.6640625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="5.5546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="5.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="5.5703125" style="1" customWidth="1"/>
     <col min="22" max="22" width="5" style="1" customWidth="1"/>
-    <col min="23" max="23" width="5.44140625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="5.21875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="4.88671875" style="1" customWidth="1"/>
-    <col min="26" max="26" width="5.33203125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="4.88671875" style="1" customWidth="1"/>
-    <col min="28" max="28" width="5.6640625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="4.6640625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="5.44140625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="4.88671875" style="1" customWidth="1"/>
-    <col min="32" max="32" width="5.6640625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="5.21875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="5.42578125" style="1" customWidth="1"/>
+    <col min="24" max="26" width="5.28515625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="5.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="5.7109375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="5" style="1" customWidth="1"/>
+    <col min="30" max="30" width="5.42578125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="5.28515625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="5.7109375" style="1" customWidth="1"/>
+    <col min="33" max="33" width="5.28515625" style="1" customWidth="1"/>
     <col min="34" max="34" width="6" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="8.88671875" style="1"/>
+    <col min="35" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="57" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="51"/>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
+    <row r="1" spans="1:51" s="38" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="32"/>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A2" s="51"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="69" t="s">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2" s="32"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71"/>
-      <c r="X2" s="71"/>
-      <c r="Y2" s="71"/>
-      <c r="Z2" s="71"/>
-      <c r="AA2" s="71"/>
-      <c r="AB2" s="71"/>
-      <c r="AC2" s="71"/>
-      <c r="AD2" s="71"/>
-      <c r="AE2" s="71"/>
-      <c r="AF2" s="71"/>
-      <c r="AG2" s="71"/>
-      <c r="AH2" s="72"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="67"/>
+      <c r="W2" s="67"/>
+      <c r="X2" s="67"/>
+      <c r="Y2" s="67"/>
+      <c r="Z2" s="67"/>
+      <c r="AA2" s="67"/>
+      <c r="AB2" s="67"/>
+      <c r="AC2" s="67"/>
+      <c r="AD2" s="67"/>
+      <c r="AE2" s="67"/>
+      <c r="AF2" s="67"/>
+      <c r="AG2" s="67"/>
+      <c r="AH2" s="68"/>
       <c r="AI2" s="2"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="33" t="s">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A3" s="32"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="27" t="s">
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="27" t="s">
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="V3" s="27"/>
-      <c r="W3" s="27"/>
-      <c r="X3" s="27"/>
-      <c r="Y3" s="27"/>
-      <c r="Z3" s="27"/>
-      <c r="AA3" s="27"/>
-      <c r="AB3" s="27"/>
-      <c r="AC3" s="27"/>
-      <c r="AD3" s="27"/>
-      <c r="AE3" s="27"/>
-      <c r="AF3" s="27"/>
-      <c r="AG3" s="27"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="65"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="85"/>
+      <c r="Z3" s="85"/>
+      <c r="AA3" s="85"/>
+      <c r="AB3" s="85"/>
+      <c r="AC3" s="85"/>
+      <c r="AD3" s="85"/>
+      <c r="AE3" s="85"/>
+      <c r="AF3" s="85"/>
+      <c r="AG3" s="85"/>
+      <c r="AH3" s="86"/>
+      <c r="AI3" s="46"/>
       <c r="AJ3" s="3"/>
       <c r="AK3" s="3"/>
       <c r="AL3" s="3"/>
@@ -1491,86 +1486,86 @@
       <c r="AO3" s="3"/>
       <c r="AP3" s="3"/>
     </row>
-    <row r="4" spans="1:51" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="74" t="s">
+    <row r="4" spans="1:51" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="40"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="75"/>
-      <c r="I4" s="76" t="s">
+      <c r="H4" s="80"/>
+      <c r="I4" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="75"/>
-      <c r="K4" s="76" t="s">
+      <c r="J4" s="80"/>
+      <c r="K4" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="75"/>
-      <c r="M4" s="76" t="s">
+      <c r="L4" s="80"/>
+      <c r="M4" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="75"/>
-      <c r="O4" s="77" t="s">
+      <c r="N4" s="80"/>
+      <c r="O4" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="76" t="s">
+      <c r="P4" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="75"/>
-      <c r="R4" s="78" t="s">
+      <c r="Q4" s="80"/>
+      <c r="R4" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="S4" s="86" t="s">
+      <c r="S4" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="87"/>
-      <c r="U4" s="81" t="s">
+      <c r="T4" s="84"/>
+      <c r="U4" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="V4" s="82" t="s">
+      <c r="V4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="W4" s="83"/>
-      <c r="X4" s="84" t="s">
+      <c r="W4" s="61"/>
+      <c r="X4" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="Y4" s="82" t="s">
+      <c r="Y4" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="Z4" s="83"/>
-      <c r="AA4" s="82" t="s">
+      <c r="Z4" s="61"/>
+      <c r="AA4" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="AB4" s="83"/>
-      <c r="AC4" s="82" t="s">
+      <c r="AB4" s="61"/>
+      <c r="AC4" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="AD4" s="83"/>
-      <c r="AE4" s="82" t="s">
+      <c r="AD4" s="61"/>
+      <c r="AE4" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="AF4" s="83"/>
-      <c r="AG4" s="82" t="s">
+      <c r="AF4" s="61"/>
+      <c r="AG4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="AH4" s="85"/>
-      <c r="AI4" s="64"/>
-      <c r="AJ4" s="51"/>
-      <c r="AK4" s="51"/>
-      <c r="AL4" s="51"/>
-      <c r="AM4" s="51"/>
-      <c r="AN4" s="51"/>
-      <c r="AO4" s="51"/>
-      <c r="AP4" s="51"/>
+      <c r="AH4" s="82"/>
+      <c r="AI4" s="45"/>
+      <c r="AJ4" s="32"/>
+      <c r="AK4" s="32"/>
+      <c r="AL4" s="32"/>
+      <c r="AM4" s="32"/>
+      <c r="AN4" s="32"/>
+      <c r="AO4" s="32"/>
+      <c r="AP4" s="32"/>
       <c r="AQ4" s="2"/>
     </row>
-    <row r="5" spans="1:51" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="61"/>
-      <c r="B5" s="62"/>
+    <row r="5" spans="1:51" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="42"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="8" t="s">
         <v>24</v>
       </c>
@@ -1583,7 +1578,7 @@
       <c r="F5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="27" t="s">
         <v>31</v>
       </c>
       <c r="H5" s="5" t="s">
@@ -1665,18 +1660,18 @@
       <c r="AH5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AI5" s="64"/>
-      <c r="AJ5" s="51"/>
-      <c r="AK5" s="51"/>
-      <c r="AL5" s="51"/>
-      <c r="AM5" s="51"/>
-      <c r="AN5" s="51"/>
-      <c r="AO5" s="51"/>
-      <c r="AP5" s="51"/>
+      <c r="AI5" s="45"/>
+      <c r="AJ5" s="32"/>
+      <c r="AK5" s="32"/>
+      <c r="AL5" s="32"/>
+      <c r="AM5" s="32"/>
+      <c r="AN5" s="32"/>
+      <c r="AO5" s="32"/>
+      <c r="AP5" s="32"/>
       <c r="AQ5" s="2"/>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A6" s="69" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -1692,7 +1687,7 @@
       <c r="F6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="38"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="16"/>
       <c r="I6" s="22"/>
       <c r="J6" s="16"/>
@@ -1720,14 +1715,14 @@
       <c r="AF6" s="16"/>
       <c r="AG6" s="22"/>
       <c r="AH6" s="17"/>
-      <c r="AI6" s="63"/>
-      <c r="AJ6" s="55"/>
-      <c r="AK6" s="55"/>
-      <c r="AL6" s="55"/>
-      <c r="AM6" s="55"/>
-      <c r="AN6" s="55"/>
-      <c r="AO6" s="55"/>
-      <c r="AP6" s="55"/>
+      <c r="AI6" s="44"/>
+      <c r="AJ6" s="36"/>
+      <c r="AK6" s="36"/>
+      <c r="AL6" s="36"/>
+      <c r="AM6" s="36"/>
+      <c r="AN6" s="36"/>
+      <c r="AO6" s="36"/>
+      <c r="AP6" s="36"/>
       <c r="AQ6" s="7"/>
       <c r="AR6" s="5"/>
       <c r="AS6" s="5"/>
@@ -1738,8 +1733,8 @@
       <c r="AX6" s="5"/>
       <c r="AY6" s="5"/>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A7" s="70"/>
       <c r="B7" s="12" t="s">
         <v>5</v>
       </c>
@@ -1753,7 +1748,7 @@
       <c r="F7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="38"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="6"/>
       <c r="I7" s="22"/>
       <c r="J7" s="6"/>
@@ -1785,14 +1780,14 @@
       <c r="AF7" s="6"/>
       <c r="AG7" s="22"/>
       <c r="AH7" s="11"/>
-      <c r="AI7" s="63"/>
-      <c r="AJ7" s="55"/>
-      <c r="AK7" s="55"/>
-      <c r="AL7" s="55"/>
-      <c r="AM7" s="55"/>
-      <c r="AN7" s="55"/>
-      <c r="AO7" s="55"/>
-      <c r="AP7" s="55"/>
+      <c r="AI7" s="44"/>
+      <c r="AJ7" s="36"/>
+      <c r="AK7" s="36"/>
+      <c r="AL7" s="36"/>
+      <c r="AM7" s="36"/>
+      <c r="AN7" s="36"/>
+      <c r="AO7" s="36"/>
+      <c r="AP7" s="36"/>
       <c r="AQ7" s="7"/>
       <c r="AR7" s="5"/>
       <c r="AS7" s="5"/>
@@ -1803,9 +1798,9 @@
       <c r="AX7" s="5"/>
       <c r="AY7" s="5"/>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A8" s="30"/>
-      <c r="B8" s="90" t="s">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A8" s="70"/>
+      <c r="B8" s="57" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="15"/>
@@ -1816,7 +1811,7 @@
       <c r="F8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="38"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="16"/>
       <c r="I8" s="22"/>
       <c r="J8" s="16"/>
@@ -1827,14 +1822,20 @@
       <c r="O8" s="16"/>
       <c r="P8" s="22"/>
       <c r="Q8" s="16"/>
-      <c r="R8" s="22"/>
+      <c r="R8" s="22" t="s">
+        <v>33</v>
+      </c>
       <c r="S8" s="16" t="s">
         <v>33</v>
       </c>
       <c r="T8" s="17"/>
       <c r="U8" s="24"/>
-      <c r="V8" s="22"/>
-      <c r="W8" s="16"/>
+      <c r="V8" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="W8" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="X8" s="16"/>
       <c r="Y8" s="22"/>
       <c r="Z8" s="16"/>
@@ -1846,14 +1847,14 @@
       <c r="AF8" s="16"/>
       <c r="AG8" s="22"/>
       <c r="AH8" s="17"/>
-      <c r="AI8" s="63"/>
-      <c r="AJ8" s="55"/>
-      <c r="AK8" s="55"/>
-      <c r="AL8" s="55"/>
-      <c r="AM8" s="55"/>
-      <c r="AN8" s="55"/>
-      <c r="AO8" s="55"/>
-      <c r="AP8" s="55"/>
+      <c r="AI8" s="44"/>
+      <c r="AJ8" s="36"/>
+      <c r="AK8" s="36"/>
+      <c r="AL8" s="36"/>
+      <c r="AM8" s="36"/>
+      <c r="AN8" s="36"/>
+      <c r="AO8" s="36"/>
+      <c r="AP8" s="36"/>
       <c r="AQ8" s="7"/>
       <c r="AR8" s="5"/>
       <c r="AS8" s="5"/>
@@ -1864,9 +1865,9 @@
       <c r="AX8" s="5"/>
       <c r="AY8" s="5"/>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A9" s="30"/>
-      <c r="B9" s="91" t="s">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A9" s="70"/>
+      <c r="B9" s="58" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="10"/>
@@ -1877,7 +1878,7 @@
       <c r="F9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="38"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="6"/>
       <c r="I9" s="22"/>
       <c r="J9" s="6"/>
@@ -1895,11 +1896,17 @@
       <c r="T9" s="17"/>
       <c r="U9" s="13"/>
       <c r="V9" s="22"/>
-      <c r="W9" s="6"/>
+      <c r="W9" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="X9" s="6"/>
       <c r="Y9" s="22"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="22"/>
+      <c r="Z9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA9" s="22" t="s">
+        <v>33</v>
+      </c>
       <c r="AB9" s="6"/>
       <c r="AC9" s="22"/>
       <c r="AD9" s="6"/>
@@ -1907,14 +1914,14 @@
       <c r="AF9" s="6"/>
       <c r="AG9" s="22"/>
       <c r="AH9" s="11"/>
-      <c r="AI9" s="63"/>
-      <c r="AJ9" s="55"/>
-      <c r="AK9" s="55"/>
-      <c r="AL9" s="55"/>
-      <c r="AM9" s="55"/>
-      <c r="AN9" s="55"/>
-      <c r="AO9" s="55"/>
-      <c r="AP9" s="55"/>
+      <c r="AI9" s="44"/>
+      <c r="AJ9" s="36"/>
+      <c r="AK9" s="36"/>
+      <c r="AL9" s="36"/>
+      <c r="AM9" s="36"/>
+      <c r="AN9" s="36"/>
+      <c r="AO9" s="36"/>
+      <c r="AP9" s="36"/>
       <c r="AQ9" s="7"/>
       <c r="AR9" s="5"/>
       <c r="AS9" s="5"/>
@@ -1925,9 +1932,9 @@
       <c r="AX9" s="5"/>
       <c r="AY9" s="5"/>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="90" t="s">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A10" s="71"/>
+      <c r="B10" s="57" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -1940,7 +1947,7 @@
       <c r="F10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="38"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="16"/>
       <c r="I10" s="22"/>
       <c r="J10" s="16"/>
@@ -1984,14 +1991,14 @@
       <c r="AH10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AI10" s="63"/>
-      <c r="AJ10" s="55"/>
-      <c r="AK10" s="55"/>
-      <c r="AL10" s="55"/>
-      <c r="AM10" s="55"/>
-      <c r="AN10" s="55"/>
-      <c r="AO10" s="55"/>
-      <c r="AP10" s="55"/>
+      <c r="AI10" s="44"/>
+      <c r="AJ10" s="36"/>
+      <c r="AK10" s="36"/>
+      <c r="AL10" s="36"/>
+      <c r="AM10" s="36"/>
+      <c r="AN10" s="36"/>
+      <c r="AO10" s="36"/>
+      <c r="AP10" s="36"/>
       <c r="AQ10" s="7"/>
       <c r="AR10" s="5"/>
       <c r="AS10" s="5"/>
@@ -2002,14 +2009,14 @@
       <c r="AX10" s="5"/>
       <c r="AY10" s="5"/>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="12"/>
       <c r="C11" s="10"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="38"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="6"/>
       <c r="I11" s="22"/>
       <c r="J11" s="6"/>
@@ -2037,14 +2044,14 @@
       <c r="AF11" s="6"/>
       <c r="AG11" s="22"/>
       <c r="AH11" s="11"/>
-      <c r="AI11" s="63"/>
-      <c r="AJ11" s="55"/>
-      <c r="AK11" s="55"/>
-      <c r="AL11" s="55"/>
-      <c r="AM11" s="55"/>
-      <c r="AN11" s="55"/>
-      <c r="AO11" s="55"/>
-      <c r="AP11" s="55"/>
+      <c r="AI11" s="44"/>
+      <c r="AJ11" s="36"/>
+      <c r="AK11" s="36"/>
+      <c r="AL11" s="36"/>
+      <c r="AM11" s="36"/>
+      <c r="AN11" s="36"/>
+      <c r="AO11" s="36"/>
+      <c r="AP11" s="36"/>
       <c r="AQ11" s="7"/>
       <c r="AR11" s="5"/>
       <c r="AS11" s="5"/>
@@ -2055,18 +2062,18 @@
       <c r="AX11" s="5"/>
       <c r="AY11" s="5"/>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A12" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="55" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="28" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -2098,14 +2105,14 @@
       <c r="AF12" s="6"/>
       <c r="AG12" s="22"/>
       <c r="AH12" s="11"/>
-      <c r="AI12" s="63"/>
-      <c r="AJ12" s="55"/>
-      <c r="AK12" s="55"/>
-      <c r="AL12" s="55"/>
-      <c r="AM12" s="55"/>
-      <c r="AN12" s="55"/>
-      <c r="AO12" s="55"/>
-      <c r="AP12" s="55"/>
+      <c r="AI12" s="44"/>
+      <c r="AJ12" s="36"/>
+      <c r="AK12" s="36"/>
+      <c r="AL12" s="36"/>
+      <c r="AM12" s="36"/>
+      <c r="AN12" s="36"/>
+      <c r="AO12" s="36"/>
+      <c r="AP12" s="36"/>
       <c r="AQ12" s="7"/>
       <c r="AR12" s="5"/>
       <c r="AS12" s="5"/>
@@ -2116,9 +2123,9 @@
       <c r="AX12" s="5"/>
       <c r="AY12" s="5"/>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A13" s="30"/>
-      <c r="B13" s="89" t="s">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A13" s="70"/>
+      <c r="B13" s="56" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="15"/>
@@ -2127,7 +2134,7 @@
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="17"/>
-      <c r="G13" s="38"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="16"/>
       <c r="I13" s="22"/>
       <c r="J13" s="16" t="s">
@@ -2161,14 +2168,14 @@
       <c r="AF13" s="16"/>
       <c r="AG13" s="22"/>
       <c r="AH13" s="17"/>
-      <c r="AI13" s="63"/>
-      <c r="AJ13" s="55"/>
-      <c r="AK13" s="55"/>
-      <c r="AL13" s="55"/>
-      <c r="AM13" s="55"/>
-      <c r="AN13" s="55"/>
-      <c r="AO13" s="55"/>
-      <c r="AP13" s="55"/>
+      <c r="AI13" s="44"/>
+      <c r="AJ13" s="36"/>
+      <c r="AK13" s="36"/>
+      <c r="AL13" s="36"/>
+      <c r="AM13" s="36"/>
+      <c r="AN13" s="36"/>
+      <c r="AO13" s="36"/>
+      <c r="AP13" s="36"/>
       <c r="AQ13" s="7"/>
       <c r="AR13" s="5"/>
       <c r="AS13" s="5"/>
@@ -2179,9 +2186,9 @@
       <c r="AX13" s="5"/>
       <c r="AY13" s="5"/>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A14" s="30"/>
-      <c r="B14" s="88" t="s">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A14" s="70"/>
+      <c r="B14" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -2192,7 +2199,7 @@
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="11"/>
-      <c r="G14" s="38"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="6"/>
       <c r="I14" s="22"/>
       <c r="J14" s="6" t="s">
@@ -2230,14 +2237,14 @@
       <c r="AF14" s="6"/>
       <c r="AG14" s="22"/>
       <c r="AH14" s="11"/>
-      <c r="AI14" s="63"/>
-      <c r="AJ14" s="55"/>
-      <c r="AK14" s="55"/>
-      <c r="AL14" s="55"/>
-      <c r="AM14" s="55"/>
-      <c r="AN14" s="55"/>
-      <c r="AO14" s="55"/>
-      <c r="AP14" s="55"/>
+      <c r="AI14" s="44"/>
+      <c r="AJ14" s="36"/>
+      <c r="AK14" s="36"/>
+      <c r="AL14" s="36"/>
+      <c r="AM14" s="36"/>
+      <c r="AN14" s="36"/>
+      <c r="AO14" s="36"/>
+      <c r="AP14" s="36"/>
       <c r="AQ14" s="7"/>
       <c r="AR14" s="5"/>
       <c r="AS14" s="5"/>
@@ -2248,9 +2255,9 @@
       <c r="AX14" s="5"/>
       <c r="AY14" s="5"/>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
-      <c r="B15" s="90" t="s">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A15" s="70"/>
+      <c r="B15" s="57" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="15" t="s">
@@ -2263,7 +2270,7 @@
       <c r="F15" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="28" t="s">
         <v>33</v>
       </c>
       <c r="H15" s="16"/>
@@ -2305,14 +2312,14 @@
       <c r="AF15" s="16"/>
       <c r="AG15" s="22"/>
       <c r="AH15" s="17"/>
-      <c r="AI15" s="63"/>
-      <c r="AJ15" s="55"/>
-      <c r="AK15" s="55"/>
-      <c r="AL15" s="55"/>
-      <c r="AM15" s="55"/>
-      <c r="AN15" s="55"/>
-      <c r="AO15" s="55"/>
-      <c r="AP15" s="55"/>
+      <c r="AI15" s="44"/>
+      <c r="AJ15" s="36"/>
+      <c r="AK15" s="36"/>
+      <c r="AL15" s="36"/>
+      <c r="AM15" s="36"/>
+      <c r="AN15" s="36"/>
+      <c r="AO15" s="36"/>
+      <c r="AP15" s="36"/>
       <c r="AQ15" s="7"/>
       <c r="AR15" s="5"/>
       <c r="AS15" s="5"/>
@@ -2323,9 +2330,9 @@
       <c r="AX15" s="5"/>
       <c r="AY15" s="5"/>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
-      <c r="B16" s="91" t="s">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A16" s="70"/>
+      <c r="B16" s="58" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -2338,7 +2345,7 @@
       <c r="F16" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="38"/>
+      <c r="G16" s="28"/>
       <c r="H16" s="6"/>
       <c r="I16" s="22" t="s">
         <v>33</v>
@@ -2378,14 +2385,14 @@
       <c r="AF16" s="6"/>
       <c r="AG16" s="22"/>
       <c r="AH16" s="11"/>
-      <c r="AI16" s="63"/>
-      <c r="AJ16" s="55"/>
-      <c r="AK16" s="55"/>
-      <c r="AL16" s="55"/>
-      <c r="AM16" s="55"/>
-      <c r="AN16" s="55"/>
-      <c r="AO16" s="55"/>
-      <c r="AP16" s="55"/>
+      <c r="AI16" s="44"/>
+      <c r="AJ16" s="36"/>
+      <c r="AK16" s="36"/>
+      <c r="AL16" s="36"/>
+      <c r="AM16" s="36"/>
+      <c r="AN16" s="36"/>
+      <c r="AO16" s="36"/>
+      <c r="AP16" s="36"/>
       <c r="AQ16" s="7"/>
       <c r="AR16" s="5"/>
       <c r="AS16" s="5"/>
@@ -2396,9 +2403,9 @@
       <c r="AX16" s="5"/>
       <c r="AY16" s="5"/>
     </row>
-    <row r="17" spans="1:51" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="32"/>
-      <c r="B17" s="92" t="s">
+    <row r="17" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="72"/>
+      <c r="B17" s="59" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="18"/>
@@ -2409,7 +2416,7 @@
       <c r="F17" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="29" t="s">
         <v>33</v>
       </c>
       <c r="H17" s="19"/>
@@ -2457,14 +2464,14 @@
         <v>33</v>
       </c>
       <c r="AH17" s="20"/>
-      <c r="AI17" s="63"/>
-      <c r="AJ17" s="55"/>
-      <c r="AK17" s="55"/>
-      <c r="AL17" s="55"/>
-      <c r="AM17" s="55"/>
-      <c r="AN17" s="55"/>
-      <c r="AO17" s="55"/>
-      <c r="AP17" s="55"/>
+      <c r="AI17" s="44"/>
+      <c r="AJ17" s="36"/>
+      <c r="AK17" s="36"/>
+      <c r="AL17" s="36"/>
+      <c r="AM17" s="36"/>
+      <c r="AN17" s="36"/>
+      <c r="AO17" s="36"/>
+      <c r="AP17" s="36"/>
       <c r="AQ17" s="7"/>
       <c r="AR17" s="5"/>
       <c r="AS17" s="5"/>
@@ -2475,163 +2482,163 @@
       <c r="AX17" s="5"/>
       <c r="AY17" s="5"/>
     </row>
-    <row r="18" spans="1:51" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="52"/>
-      <c r="N18" s="52"/>
-      <c r="O18" s="52"/>
-      <c r="P18" s="52"/>
-      <c r="Q18" s="52"/>
-      <c r="R18" s="52"/>
-      <c r="S18" s="52"/>
-      <c r="T18" s="52"/>
-      <c r="U18" s="52"/>
-      <c r="V18" s="52"/>
-      <c r="W18" s="52"/>
-      <c r="X18" s="52"/>
-      <c r="Y18" s="52"/>
-      <c r="Z18" s="52"/>
-      <c r="AA18" s="52"/>
-      <c r="AB18" s="52"/>
-      <c r="AC18" s="52"/>
-      <c r="AD18" s="52"/>
-      <c r="AE18" s="52"/>
-      <c r="AF18" s="52"/>
-      <c r="AG18" s="52"/>
-      <c r="AH18" s="52"/>
-      <c r="AI18" s="55"/>
-      <c r="AJ18" s="55"/>
-      <c r="AK18" s="55"/>
-      <c r="AL18" s="55"/>
-      <c r="AM18" s="55"/>
-      <c r="AN18" s="55"/>
-      <c r="AO18" s="55"/>
-      <c r="AP18" s="55"/>
-      <c r="AQ18" s="53"/>
-      <c r="AR18" s="53"/>
-      <c r="AS18" s="53"/>
-      <c r="AT18" s="53"/>
-      <c r="AU18" s="53"/>
-      <c r="AV18" s="53"/>
-      <c r="AW18" s="53"/>
-      <c r="AX18" s="53"/>
-      <c r="AY18" s="53"/>
+    <row r="18" spans="1:51" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
+      <c r="U18" s="33"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="33"/>
+      <c r="X18" s="33"/>
+      <c r="Y18" s="33"/>
+      <c r="Z18" s="33"/>
+      <c r="AA18" s="33"/>
+      <c r="AB18" s="33"/>
+      <c r="AC18" s="33"/>
+      <c r="AD18" s="33"/>
+      <c r="AE18" s="33"/>
+      <c r="AF18" s="33"/>
+      <c r="AG18" s="33"/>
+      <c r="AH18" s="33"/>
+      <c r="AI18" s="36"/>
+      <c r="AJ18" s="36"/>
+      <c r="AK18" s="36"/>
+      <c r="AL18" s="36"/>
+      <c r="AM18" s="36"/>
+      <c r="AN18" s="36"/>
+      <c r="AO18" s="36"/>
+      <c r="AP18" s="36"/>
+      <c r="AQ18" s="34"/>
+      <c r="AR18" s="34"/>
+      <c r="AS18" s="34"/>
+      <c r="AT18" s="34"/>
+      <c r="AU18" s="34"/>
+      <c r="AV18" s="34"/>
+      <c r="AW18" s="34"/>
+      <c r="AX18" s="34"/>
+      <c r="AY18" s="34"/>
     </row>
-    <row r="19" spans="1:51" s="57" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="68" t="s">
+    <row r="19" spans="1:51" s="38" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="55"/>
-      <c r="L19" s="55"/>
-      <c r="M19" s="55"/>
-      <c r="N19" s="55"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="55"/>
-      <c r="R19" s="55"/>
-      <c r="S19" s="55"/>
-      <c r="T19" s="55"/>
-      <c r="U19" s="55"/>
-      <c r="V19" s="55"/>
-      <c r="W19" s="55"/>
-      <c r="X19" s="55"/>
-      <c r="Y19" s="55"/>
-      <c r="Z19" s="55"/>
-      <c r="AA19" s="55"/>
-      <c r="AB19" s="55"/>
-      <c r="AC19" s="55"/>
-      <c r="AD19" s="55"/>
-      <c r="AE19" s="55"/>
-      <c r="AF19" s="55"/>
-      <c r="AG19" s="55"/>
-      <c r="AH19" s="55"/>
-      <c r="AI19" s="55"/>
-      <c r="AJ19" s="55"/>
-      <c r="AK19" s="55"/>
-      <c r="AL19" s="55"/>
-      <c r="AM19" s="55"/>
-      <c r="AN19" s="55"/>
-      <c r="AO19" s="55"/>
-      <c r="AP19" s="55"/>
-      <c r="AQ19" s="55"/>
-      <c r="AR19" s="55"/>
-      <c r="AS19" s="56"/>
-      <c r="AT19" s="56"/>
-      <c r="AU19" s="56"/>
-      <c r="AV19" s="56"/>
-      <c r="AW19" s="56"/>
-      <c r="AX19" s="56"/>
-      <c r="AY19" s="56"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="88"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="36"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="36"/>
+      <c r="U19" s="36"/>
+      <c r="V19" s="36"/>
+      <c r="W19" s="36"/>
+      <c r="X19" s="36"/>
+      <c r="Y19" s="36"/>
+      <c r="Z19" s="36"/>
+      <c r="AA19" s="36"/>
+      <c r="AB19" s="36"/>
+      <c r="AC19" s="36"/>
+      <c r="AD19" s="36"/>
+      <c r="AE19" s="36"/>
+      <c r="AF19" s="36"/>
+      <c r="AG19" s="36"/>
+      <c r="AH19" s="36"/>
+      <c r="AI19" s="36"/>
+      <c r="AJ19" s="36"/>
+      <c r="AK19" s="36"/>
+      <c r="AL19" s="36"/>
+      <c r="AM19" s="36"/>
+      <c r="AN19" s="36"/>
+      <c r="AO19" s="36"/>
+      <c r="AP19" s="36"/>
+      <c r="AQ19" s="36"/>
+      <c r="AR19" s="36"/>
+      <c r="AS19" s="37"/>
+      <c r="AT19" s="37"/>
+      <c r="AU19" s="37"/>
+      <c r="AV19" s="37"/>
+      <c r="AW19" s="37"/>
+      <c r="AX19" s="37"/>
+      <c r="AY19" s="37"/>
     </row>
-    <row r="20" spans="1:51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="42"/>
-      <c r="B20" s="43" t="s">
+    <row r="20" spans="1:51" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="30"/>
+      <c r="B20" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="43" t="s">
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="N20" s="43"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="43"/>
-      <c r="Q20" s="43"/>
-      <c r="R20" s="43"/>
-      <c r="S20" s="43"/>
-      <c r="T20" s="43"/>
-      <c r="U20" s="43"/>
-      <c r="V20" s="43"/>
-      <c r="W20" s="43"/>
-      <c r="X20" s="43"/>
-      <c r="Y20" s="43"/>
-      <c r="Z20" s="43"/>
-      <c r="AA20" s="63"/>
-      <c r="AB20" s="55"/>
-      <c r="AC20" s="55"/>
-      <c r="AD20" s="55"/>
-      <c r="AE20" s="55"/>
-      <c r="AF20" s="55"/>
-      <c r="AG20" s="55"/>
-      <c r="AH20" s="55"/>
-      <c r="AI20" s="55"/>
-      <c r="AJ20" s="55"/>
-      <c r="AK20" s="55"/>
-      <c r="AL20" s="55"/>
-      <c r="AM20" s="55"/>
-      <c r="AN20" s="55"/>
-      <c r="AO20" s="55"/>
-      <c r="AP20" s="55"/>
-      <c r="AQ20" s="55"/>
-      <c r="AR20" s="55"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="63"/>
+      <c r="R20" s="63"/>
+      <c r="S20" s="63"/>
+      <c r="T20" s="63"/>
+      <c r="U20" s="63"/>
+      <c r="V20" s="63"/>
+      <c r="W20" s="63"/>
+      <c r="X20" s="63"/>
+      <c r="Y20" s="63"/>
+      <c r="Z20" s="63"/>
+      <c r="AA20" s="44"/>
+      <c r="AB20" s="36"/>
+      <c r="AC20" s="36"/>
+      <c r="AD20" s="36"/>
+      <c r="AE20" s="36"/>
+      <c r="AF20" s="36"/>
+      <c r="AG20" s="36"/>
+      <c r="AH20" s="36"/>
+      <c r="AI20" s="36"/>
+      <c r="AJ20" s="36"/>
+      <c r="AK20" s="36"/>
+      <c r="AL20" s="36"/>
+      <c r="AM20" s="36"/>
+      <c r="AN20" s="36"/>
+      <c r="AO20" s="36"/>
+      <c r="AP20" s="36"/>
+      <c r="AQ20" s="36"/>
+      <c r="AR20" s="36"/>
       <c r="AS20" s="7"/>
       <c r="AT20" s="5"/>
       <c r="AU20" s="5"/>
@@ -2640,55 +2647,55 @@
       <c r="AX20" s="5"/>
       <c r="AY20" s="5"/>
     </row>
-    <row r="21" spans="1:51" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="44" t="s">
+    <row r="21" spans="1:51" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="50"/>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="50"/>
-      <c r="S21" s="50"/>
-      <c r="T21" s="50"/>
-      <c r="U21" s="50"/>
-      <c r="V21" s="50"/>
-      <c r="W21" s="50"/>
-      <c r="X21" s="50"/>
-      <c r="Y21" s="50"/>
-      <c r="Z21" s="50"/>
-      <c r="AA21" s="63"/>
-      <c r="AB21" s="55"/>
-      <c r="AC21" s="55"/>
-      <c r="AD21" s="55"/>
-      <c r="AE21" s="55"/>
-      <c r="AF21" s="55"/>
-      <c r="AG21" s="55"/>
-      <c r="AH21" s="55"/>
-      <c r="AI21" s="55"/>
-      <c r="AJ21" s="55"/>
-      <c r="AK21" s="55"/>
-      <c r="AL21" s="55"/>
-      <c r="AM21" s="55"/>
-      <c r="AN21" s="55"/>
-      <c r="AO21" s="55"/>
-      <c r="AP21" s="55"/>
-      <c r="AQ21" s="55"/>
-      <c r="AR21" s="55"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="62"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="90"/>
+      <c r="N21" s="90"/>
+      <c r="O21" s="90"/>
+      <c r="P21" s="90"/>
+      <c r="Q21" s="90"/>
+      <c r="R21" s="90"/>
+      <c r="S21" s="90"/>
+      <c r="T21" s="90"/>
+      <c r="U21" s="90"/>
+      <c r="V21" s="90"/>
+      <c r="W21" s="90"/>
+      <c r="X21" s="90"/>
+      <c r="Y21" s="90"/>
+      <c r="Z21" s="90"/>
+      <c r="AA21" s="44"/>
+      <c r="AB21" s="36"/>
+      <c r="AC21" s="36"/>
+      <c r="AD21" s="36"/>
+      <c r="AE21" s="36"/>
+      <c r="AF21" s="36"/>
+      <c r="AG21" s="36"/>
+      <c r="AH21" s="36"/>
+      <c r="AI21" s="36"/>
+      <c r="AJ21" s="36"/>
+      <c r="AK21" s="36"/>
+      <c r="AL21" s="36"/>
+      <c r="AM21" s="36"/>
+      <c r="AN21" s="36"/>
+      <c r="AO21" s="36"/>
+      <c r="AP21" s="36"/>
+      <c r="AQ21" s="36"/>
+      <c r="AR21" s="36"/>
       <c r="AS21" s="7"/>
       <c r="AT21" s="5"/>
       <c r="AU21" s="5"/>
@@ -2697,55 +2704,55 @@
       <c r="AX21" s="5"/>
       <c r="AY21" s="5"/>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A22" s="73" t="s">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A22" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="46" t="s">
+      <c r="B22" s="64"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
-      <c r="P22" s="46"/>
-      <c r="Q22" s="46"/>
-      <c r="R22" s="46"/>
-      <c r="S22" s="46"/>
-      <c r="T22" s="46"/>
-      <c r="U22" s="46"/>
-      <c r="V22" s="46"/>
-      <c r="W22" s="46"/>
-      <c r="X22" s="46"/>
-      <c r="Y22" s="46"/>
-      <c r="Z22" s="46"/>
-      <c r="AA22" s="63"/>
-      <c r="AB22" s="55"/>
-      <c r="AC22" s="55"/>
-      <c r="AD22" s="55"/>
-      <c r="AE22" s="55"/>
-      <c r="AF22" s="55"/>
-      <c r="AG22" s="55"/>
-      <c r="AH22" s="55"/>
-      <c r="AI22" s="55"/>
-      <c r="AJ22" s="55"/>
-      <c r="AK22" s="55"/>
-      <c r="AL22" s="55"/>
-      <c r="AM22" s="55"/>
-      <c r="AN22" s="55"/>
-      <c r="AO22" s="55"/>
-      <c r="AP22" s="55"/>
-      <c r="AQ22" s="55"/>
-      <c r="AR22" s="55"/>
+      <c r="N22" s="91"/>
+      <c r="O22" s="91"/>
+      <c r="P22" s="91"/>
+      <c r="Q22" s="91"/>
+      <c r="R22" s="91"/>
+      <c r="S22" s="91"/>
+      <c r="T22" s="91"/>
+      <c r="U22" s="91"/>
+      <c r="V22" s="91"/>
+      <c r="W22" s="91"/>
+      <c r="X22" s="91"/>
+      <c r="Y22" s="91"/>
+      <c r="Z22" s="91"/>
+      <c r="AA22" s="44"/>
+      <c r="AB22" s="36"/>
+      <c r="AC22" s="36"/>
+      <c r="AD22" s="36"/>
+      <c r="AE22" s="36"/>
+      <c r="AF22" s="36"/>
+      <c r="AG22" s="36"/>
+      <c r="AH22" s="36"/>
+      <c r="AI22" s="36"/>
+      <c r="AJ22" s="36"/>
+      <c r="AK22" s="36"/>
+      <c r="AL22" s="36"/>
+      <c r="AM22" s="36"/>
+      <c r="AN22" s="36"/>
+      <c r="AO22" s="36"/>
+      <c r="AP22" s="36"/>
+      <c r="AQ22" s="36"/>
+      <c r="AR22" s="36"/>
       <c r="AS22" s="7"/>
       <c r="AT22" s="5"/>
       <c r="AU22" s="5"/>
@@ -2754,406 +2761,406 @@
       <c r="AX22" s="5"/>
       <c r="AY22" s="5"/>
     </row>
-    <row r="23" spans="1:51" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="73" t="s">
+    <row r="23" spans="1:51" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="46" t="s">
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="N23" s="46"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="46"/>
-      <c r="S23" s="46"/>
-      <c r="T23" s="46"/>
-      <c r="U23" s="46"/>
-      <c r="V23" s="46"/>
-      <c r="W23" s="46"/>
-      <c r="X23" s="46"/>
-      <c r="Y23" s="46"/>
-      <c r="Z23" s="46"/>
-      <c r="AA23" s="64"/>
-      <c r="AB23" s="51"/>
-      <c r="AC23" s="51"/>
-      <c r="AD23" s="51"/>
-      <c r="AE23" s="51"/>
-      <c r="AF23" s="51"/>
-      <c r="AG23" s="51"/>
-      <c r="AH23" s="51"/>
-      <c r="AI23" s="51"/>
-      <c r="AJ23" s="51"/>
-      <c r="AK23" s="51"/>
-      <c r="AL23" s="51"/>
-      <c r="AM23" s="51"/>
-      <c r="AN23" s="51"/>
-      <c r="AO23" s="51"/>
-      <c r="AP23" s="51"/>
-      <c r="AQ23" s="51"/>
-      <c r="AR23" s="51"/>
+      <c r="N23" s="91"/>
+      <c r="O23" s="91"/>
+      <c r="P23" s="91"/>
+      <c r="Q23" s="91"/>
+      <c r="R23" s="91"/>
+      <c r="S23" s="91"/>
+      <c r="T23" s="91"/>
+      <c r="U23" s="91"/>
+      <c r="V23" s="91"/>
+      <c r="W23" s="91"/>
+      <c r="X23" s="91"/>
+      <c r="Y23" s="91"/>
+      <c r="Z23" s="91"/>
+      <c r="AA23" s="45"/>
+      <c r="AB23" s="32"/>
+      <c r="AC23" s="32"/>
+      <c r="AD23" s="32"/>
+      <c r="AE23" s="32"/>
+      <c r="AF23" s="32"/>
+      <c r="AG23" s="32"/>
+      <c r="AH23" s="32"/>
+      <c r="AI23" s="32"/>
+      <c r="AJ23" s="32"/>
+      <c r="AK23" s="32"/>
+      <c r="AL23" s="32"/>
+      <c r="AM23" s="32"/>
+      <c r="AN23" s="32"/>
+      <c r="AO23" s="32"/>
+      <c r="AP23" s="32"/>
+      <c r="AQ23" s="32"/>
+      <c r="AR23" s="32"/>
       <c r="AS23" s="2"/>
     </row>
-    <row r="24" spans="1:51" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="73" t="s">
+    <row r="24" spans="1:51" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="46" t="s">
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
-      <c r="P24" s="46"/>
-      <c r="Q24" s="46"/>
-      <c r="R24" s="46"/>
-      <c r="S24" s="46"/>
-      <c r="T24" s="46"/>
-      <c r="U24" s="46"/>
-      <c r="V24" s="46"/>
-      <c r="W24" s="46"/>
-      <c r="X24" s="46"/>
-      <c r="Y24" s="46"/>
-      <c r="Z24" s="46"/>
-      <c r="AA24" s="64"/>
-      <c r="AB24" s="51"/>
-      <c r="AC24" s="51"/>
-      <c r="AD24" s="51"/>
-      <c r="AE24" s="51"/>
-      <c r="AF24" s="51"/>
-      <c r="AG24" s="51"/>
-      <c r="AH24" s="51"/>
-      <c r="AI24" s="51"/>
-      <c r="AJ24" s="51"/>
-      <c r="AK24" s="51"/>
-      <c r="AL24" s="51"/>
-      <c r="AM24" s="51"/>
-      <c r="AN24" s="51"/>
-      <c r="AO24" s="51"/>
-      <c r="AP24" s="51"/>
-      <c r="AQ24" s="51"/>
-      <c r="AR24" s="51"/>
+      <c r="N24" s="91"/>
+      <c r="O24" s="91"/>
+      <c r="P24" s="91"/>
+      <c r="Q24" s="91"/>
+      <c r="R24" s="91"/>
+      <c r="S24" s="91"/>
+      <c r="T24" s="91"/>
+      <c r="U24" s="91"/>
+      <c r="V24" s="91"/>
+      <c r="W24" s="91"/>
+      <c r="X24" s="91"/>
+      <c r="Y24" s="91"/>
+      <c r="Z24" s="91"/>
+      <c r="AA24" s="45"/>
+      <c r="AB24" s="32"/>
+      <c r="AC24" s="32"/>
+      <c r="AD24" s="32"/>
+      <c r="AE24" s="32"/>
+      <c r="AF24" s="32"/>
+      <c r="AG24" s="32"/>
+      <c r="AH24" s="32"/>
+      <c r="AI24" s="32"/>
+      <c r="AJ24" s="32"/>
+      <c r="AK24" s="32"/>
+      <c r="AL24" s="32"/>
+      <c r="AM24" s="32"/>
+      <c r="AN24" s="32"/>
+      <c r="AO24" s="32"/>
+      <c r="AP24" s="32"/>
+      <c r="AQ24" s="32"/>
+      <c r="AR24" s="32"/>
       <c r="AS24" s="2"/>
     </row>
-    <row r="25" spans="1:51" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="44" t="s">
+    <row r="25" spans="1:51" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="50"/>
-      <c r="O25" s="50"/>
-      <c r="P25" s="50"/>
-      <c r="Q25" s="50"/>
-      <c r="R25" s="50"/>
-      <c r="S25" s="50"/>
-      <c r="T25" s="50"/>
-      <c r="U25" s="50"/>
-      <c r="V25" s="50"/>
-      <c r="W25" s="50"/>
-      <c r="X25" s="50"/>
-      <c r="Y25" s="50"/>
-      <c r="Z25" s="50"/>
-      <c r="AA25" s="64"/>
-      <c r="AB25" s="51"/>
-      <c r="AC25" s="51"/>
-      <c r="AD25" s="51"/>
-      <c r="AE25" s="51"/>
-      <c r="AF25" s="51"/>
-      <c r="AG25" s="51"/>
-      <c r="AH25" s="51"/>
-      <c r="AI25" s="51"/>
-      <c r="AJ25" s="51"/>
-      <c r="AK25" s="51"/>
-      <c r="AL25" s="51"/>
-      <c r="AM25" s="51"/>
-      <c r="AN25" s="51"/>
-      <c r="AO25" s="51"/>
-      <c r="AP25" s="51"/>
-      <c r="AQ25" s="51"/>
-      <c r="AR25" s="51"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="90"/>
+      <c r="N25" s="90"/>
+      <c r="O25" s="90"/>
+      <c r="P25" s="90"/>
+      <c r="Q25" s="90"/>
+      <c r="R25" s="90"/>
+      <c r="S25" s="90"/>
+      <c r="T25" s="90"/>
+      <c r="U25" s="90"/>
+      <c r="V25" s="90"/>
+      <c r="W25" s="90"/>
+      <c r="X25" s="90"/>
+      <c r="Y25" s="90"/>
+      <c r="Z25" s="90"/>
+      <c r="AA25" s="45"/>
+      <c r="AB25" s="32"/>
+      <c r="AC25" s="32"/>
+      <c r="AD25" s="32"/>
+      <c r="AE25" s="32"/>
+      <c r="AF25" s="32"/>
+      <c r="AG25" s="32"/>
+      <c r="AH25" s="32"/>
+      <c r="AI25" s="32"/>
+      <c r="AJ25" s="32"/>
+      <c r="AK25" s="32"/>
+      <c r="AL25" s="32"/>
+      <c r="AM25" s="32"/>
+      <c r="AN25" s="32"/>
+      <c r="AO25" s="32"/>
+      <c r="AP25" s="32"/>
+      <c r="AQ25" s="32"/>
+      <c r="AR25" s="32"/>
       <c r="AS25" s="2"/>
     </row>
-    <row r="26" spans="1:51" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="79" t="s">
+    <row r="26" spans="1:51" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="46" t="s">
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="62"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="N26" s="46"/>
-      <c r="O26" s="46"/>
-      <c r="P26" s="46"/>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="46"/>
-      <c r="S26" s="46"/>
-      <c r="T26" s="46"/>
-      <c r="U26" s="46"/>
-      <c r="V26" s="46"/>
-      <c r="W26" s="46"/>
-      <c r="X26" s="46"/>
-      <c r="Y26" s="46"/>
-      <c r="Z26" s="46"/>
-      <c r="AA26" s="64"/>
-      <c r="AB26" s="51"/>
-      <c r="AC26" s="51"/>
-      <c r="AD26" s="51"/>
-      <c r="AE26" s="51"/>
-      <c r="AF26" s="51"/>
-      <c r="AG26" s="51"/>
-      <c r="AH26" s="51"/>
-      <c r="AI26" s="51"/>
-      <c r="AJ26" s="51"/>
-      <c r="AK26" s="51"/>
-      <c r="AL26" s="51"/>
-      <c r="AM26" s="51"/>
-      <c r="AN26" s="51"/>
-      <c r="AO26" s="51"/>
-      <c r="AP26" s="51"/>
-      <c r="AQ26" s="51"/>
-      <c r="AR26" s="51"/>
+      <c r="N26" s="91"/>
+      <c r="O26" s="91"/>
+      <c r="P26" s="91"/>
+      <c r="Q26" s="91"/>
+      <c r="R26" s="91"/>
+      <c r="S26" s="91"/>
+      <c r="T26" s="91"/>
+      <c r="U26" s="91"/>
+      <c r="V26" s="91"/>
+      <c r="W26" s="91"/>
+      <c r="X26" s="91"/>
+      <c r="Y26" s="91"/>
+      <c r="Z26" s="91"/>
+      <c r="AA26" s="45"/>
+      <c r="AB26" s="32"/>
+      <c r="AC26" s="32"/>
+      <c r="AD26" s="32"/>
+      <c r="AE26" s="32"/>
+      <c r="AF26" s="32"/>
+      <c r="AG26" s="32"/>
+      <c r="AH26" s="32"/>
+      <c r="AI26" s="32"/>
+      <c r="AJ26" s="32"/>
+      <c r="AK26" s="32"/>
+      <c r="AL26" s="32"/>
+      <c r="AM26" s="32"/>
+      <c r="AN26" s="32"/>
+      <c r="AO26" s="32"/>
+      <c r="AP26" s="32"/>
+      <c r="AQ26" s="32"/>
+      <c r="AR26" s="32"/>
       <c r="AS26" s="2"/>
     </row>
-    <row r="27" spans="1:51" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="79" t="s">
+    <row r="27" spans="1:51" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="45"/>
-      <c r="M27" s="46" t="s">
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="N27" s="46"/>
-      <c r="O27" s="46"/>
-      <c r="P27" s="46"/>
-      <c r="Q27" s="46"/>
-      <c r="R27" s="46"/>
-      <c r="S27" s="46"/>
-      <c r="T27" s="46"/>
-      <c r="U27" s="46"/>
-      <c r="V27" s="46"/>
-      <c r="W27" s="46"/>
-      <c r="X27" s="46"/>
-      <c r="Y27" s="46"/>
-      <c r="Z27" s="46"/>
-      <c r="AA27" s="64"/>
-      <c r="AB27" s="51"/>
-      <c r="AC27" s="51"/>
-      <c r="AD27" s="51"/>
-      <c r="AE27" s="51"/>
-      <c r="AF27" s="51"/>
-      <c r="AG27" s="51"/>
-      <c r="AH27" s="51"/>
-      <c r="AI27" s="51"/>
-      <c r="AJ27" s="51"/>
-      <c r="AK27" s="51"/>
-      <c r="AL27" s="51"/>
-      <c r="AM27" s="51"/>
-      <c r="AN27" s="51"/>
-      <c r="AO27" s="51"/>
-      <c r="AP27" s="51"/>
-      <c r="AQ27" s="51"/>
-      <c r="AR27" s="51"/>
+      <c r="N27" s="91"/>
+      <c r="O27" s="91"/>
+      <c r="P27" s="91"/>
+      <c r="Q27" s="91"/>
+      <c r="R27" s="91"/>
+      <c r="S27" s="91"/>
+      <c r="T27" s="91"/>
+      <c r="U27" s="91"/>
+      <c r="V27" s="91"/>
+      <c r="W27" s="91"/>
+      <c r="X27" s="91"/>
+      <c r="Y27" s="91"/>
+      <c r="Z27" s="91"/>
+      <c r="AA27" s="45"/>
+      <c r="AB27" s="32"/>
+      <c r="AC27" s="32"/>
+      <c r="AD27" s="32"/>
+      <c r="AE27" s="32"/>
+      <c r="AF27" s="32"/>
+      <c r="AG27" s="32"/>
+      <c r="AH27" s="32"/>
+      <c r="AI27" s="32"/>
+      <c r="AJ27" s="32"/>
+      <c r="AK27" s="32"/>
+      <c r="AL27" s="32"/>
+      <c r="AM27" s="32"/>
+      <c r="AN27" s="32"/>
+      <c r="AO27" s="32"/>
+      <c r="AP27" s="32"/>
+      <c r="AQ27" s="32"/>
+      <c r="AR27" s="32"/>
       <c r="AS27" s="2"/>
     </row>
-    <row r="28" spans="1:51" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="80" t="s">
+    <row r="28" spans="1:51" ht="59.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="47"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="48" t="s">
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="89"/>
+      <c r="I28" s="89"/>
+      <c r="J28" s="89"/>
+      <c r="K28" s="89"/>
+      <c r="L28" s="89"/>
+      <c r="M28" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="N28" s="48"/>
-      <c r="O28" s="48"/>
-      <c r="P28" s="48"/>
-      <c r="Q28" s="48"/>
-      <c r="R28" s="48"/>
-      <c r="S28" s="48"/>
-      <c r="T28" s="48"/>
-      <c r="U28" s="48"/>
-      <c r="V28" s="48"/>
-      <c r="W28" s="48"/>
-      <c r="X28" s="48"/>
-      <c r="Y28" s="48"/>
-      <c r="Z28" s="48"/>
-      <c r="AA28" s="64"/>
-      <c r="AB28" s="51"/>
-      <c r="AC28" s="51"/>
-      <c r="AD28" s="51"/>
-      <c r="AE28" s="51"/>
-      <c r="AF28" s="51"/>
-      <c r="AG28" s="51"/>
-      <c r="AH28" s="51"/>
-      <c r="AI28" s="51"/>
-      <c r="AJ28" s="51"/>
-      <c r="AK28" s="51"/>
-      <c r="AL28" s="51"/>
-      <c r="AM28" s="51"/>
-      <c r="AN28" s="51"/>
-      <c r="AO28" s="51"/>
-      <c r="AP28" s="51"/>
-      <c r="AQ28" s="51"/>
-      <c r="AR28" s="51"/>
+      <c r="N28" s="92"/>
+      <c r="O28" s="92"/>
+      <c r="P28" s="92"/>
+      <c r="Q28" s="92"/>
+      <c r="R28" s="92"/>
+      <c r="S28" s="92"/>
+      <c r="T28" s="92"/>
+      <c r="U28" s="92"/>
+      <c r="V28" s="92"/>
+      <c r="W28" s="92"/>
+      <c r="X28" s="92"/>
+      <c r="Y28" s="92"/>
+      <c r="Z28" s="92"/>
+      <c r="AA28" s="45"/>
+      <c r="AB28" s="32"/>
+      <c r="AC28" s="32"/>
+      <c r="AD28" s="32"/>
+      <c r="AE28" s="32"/>
+      <c r="AF28" s="32"/>
+      <c r="AG28" s="32"/>
+      <c r="AH28" s="32"/>
+      <c r="AI28" s="32"/>
+      <c r="AJ28" s="32"/>
+      <c r="AK28" s="32"/>
+      <c r="AL28" s="32"/>
+      <c r="AM28" s="32"/>
+      <c r="AN28" s="32"/>
+      <c r="AO28" s="32"/>
+      <c r="AP28" s="32"/>
+      <c r="AQ28" s="32"/>
+      <c r="AR28" s="32"/>
       <c r="AS28" s="2"/>
     </row>
-    <row r="29" spans="1:51" s="54" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="51"/>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="51"/>
-      <c r="P29" s="51"/>
-      <c r="Q29" s="51"/>
-      <c r="R29" s="51"/>
-      <c r="S29" s="51"/>
-      <c r="T29" s="51"/>
-      <c r="U29" s="51"/>
-      <c r="V29" s="51"/>
-      <c r="W29" s="51"/>
-      <c r="X29" s="51"/>
-      <c r="Y29" s="51"/>
-      <c r="Z29" s="51"/>
-      <c r="AA29" s="51"/>
-      <c r="AB29" s="51"/>
-      <c r="AC29" s="51"/>
-      <c r="AD29" s="51"/>
-      <c r="AE29" s="51"/>
-      <c r="AF29" s="51"/>
-      <c r="AG29" s="51"/>
-      <c r="AH29" s="51"/>
-      <c r="AI29" s="51"/>
-      <c r="AJ29" s="51"/>
-      <c r="AK29" s="51"/>
-      <c r="AL29" s="51"/>
-      <c r="AM29" s="51"/>
-      <c r="AN29" s="51"/>
-      <c r="AO29" s="51"/>
-      <c r="AP29" s="51"/>
-      <c r="AQ29" s="51"/>
-      <c r="AR29" s="51"/>
+    <row r="29" spans="1:51" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="32"/>
+      <c r="Q29" s="32"/>
+      <c r="R29" s="32"/>
+      <c r="S29" s="32"/>
+      <c r="T29" s="32"/>
+      <c r="U29" s="32"/>
+      <c r="V29" s="32"/>
+      <c r="W29" s="32"/>
+      <c r="X29" s="32"/>
+      <c r="Y29" s="32"/>
+      <c r="Z29" s="32"/>
+      <c r="AA29" s="32"/>
+      <c r="AB29" s="32"/>
+      <c r="AC29" s="32"/>
+      <c r="AD29" s="32"/>
+      <c r="AE29" s="32"/>
+      <c r="AF29" s="32"/>
+      <c r="AG29" s="32"/>
+      <c r="AH29" s="32"/>
+      <c r="AI29" s="32"/>
+      <c r="AJ29" s="32"/>
+      <c r="AK29" s="32"/>
+      <c r="AL29" s="32"/>
+      <c r="AM29" s="32"/>
+      <c r="AN29" s="32"/>
+      <c r="AO29" s="32"/>
+      <c r="AP29" s="32"/>
+      <c r="AQ29" s="32"/>
+      <c r="AR29" s="32"/>
     </row>
-    <row r="30" spans="1:51" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:51" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:51" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="33" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="34" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="35" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="36" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="37" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="38" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="39" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="40" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="41" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="42" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="43" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="45" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="46" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="66" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="66" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="66" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="66" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="66" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="66" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="66" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="66" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="66" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="66" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="66" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:51" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:51" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:51" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="47" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
     <mergeCell ref="A19:F19"/>

</xml_diff>